<commit_message>
fix expot to api
</commit_message>
<xml_diff>
--- a/New folder/project-root/public/data.xlsx
+++ b/New folder/project-root/public/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t xml:space="preserve"> id</t>
   </si>
@@ -26,16 +26,19 @@
     <t>Email.</t>
   </si>
   <si>
-    <t>omar</t>
-  </si>
-  <si>
-    <t>omar@gmail.com</t>
-  </si>
-  <si>
-    <t>saif</t>
-  </si>
-  <si>
-    <t>saif@gmail.com</t>
+    <t>kahal</t>
+  </si>
+  <si>
+    <t>kahal@gmail.com</t>
+  </si>
+  <si>
+    <t>kaaaaaaaahal@gmail.com</t>
+  </si>
+  <si>
+    <t>omarrrrrrrrrrrrrrr</t>
+  </si>
+  <si>
+    <t>wq@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +399,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -407,13 +410,24 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>